<commit_message>
+ Push Added TS and TC (Seller - Negotiate Product) on Seller - Website
</commit_message>
<xml_diff>
--- a/Website - Seller .xlsx
+++ b/Website - Seller .xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="245">
   <si>
     <t>No</t>
   </si>
@@ -738,6 +738,21 @@
   <si>
     <t xml:space="preserve">User has clicked on the "Status" button </t>
   </si>
+  <si>
+    <t>TC.Nego.005</t>
+  </si>
+  <si>
+    <t>User want to update the negotiation status of products that the transaction is cancelled</t>
+  </si>
+  <si>
+    <t>To ensure that user can update the status of products that the transaction is cancelled and and on the home page, the product can be renegotiated by the user or other buyers</t>
+  </si>
+  <si>
+    <t>User select and click on the "Batalkan transaksi" options</t>
+  </si>
+  <si>
+    <t>The product status is updated to transaction is cancelled and the product can be renegotiated by user or other buyers</t>
+  </si>
 </sst>
 </file>
 
@@ -890,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1110,6 +1125,12 @@
     </xf>
     <xf borderId="7" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -32699,13 +32720,13 @@
       <c r="G46" s="58">
         <v>1.0</v>
       </c>
-      <c r="H46" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="I46" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="J46" s="60" t="s">
+      <c r="H46" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="I46" s="77" t="s">
+        <v>57</v>
+      </c>
+      <c r="J46" s="77" t="s">
         <v>17</v>
       </c>
     </row>
@@ -59600,44 +59621,96 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="48"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="71"/>
+      <c r="A15" s="49">
+        <v>5.0</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>240</v>
+      </c>
+      <c r="E15" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="F15" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="G15" s="52">
+        <v>1.0</v>
+      </c>
+      <c r="H15" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="54" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="48"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="71"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="54">
+        <v>2.0</v>
+      </c>
+      <c r="H16" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="I16" s="54" t="s">
+        <v>219</v>
+      </c>
+      <c r="J16" s="54" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="71"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="54">
+        <v>3.0</v>
+      </c>
+      <c r="H17" s="53" t="s">
+        <v>235</v>
+      </c>
+      <c r="I17" s="54" t="s">
+        <v>236</v>
+      </c>
+      <c r="J17" s="67" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="48"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="71"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="67">
+        <v>4.0</v>
+      </c>
+      <c r="H18" s="68" t="s">
+        <v>243</v>
+      </c>
+      <c r="I18" s="67" t="s">
+        <v>244</v>
+      </c>
+      <c r="J18" s="67" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="48"/>
@@ -67990,7 +68063,7 @@
       <c r="H853" s="71"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="30">
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="A2:A4"/>
@@ -68008,6 +68081,12 @@
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="E8:E10"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="C11:C14"/>

</xml_diff>